<commit_message>
Finished overall project review for PCB fabrication at JLCPCB.
</commit_message>
<xml_diff>
--- a/HARDWARE/KICAD/FABRICATION/JLCPCB/EMBARCADOS - CURSO PCB - BOM (JLCPCB).xlsx
+++ b/HARDWARE/KICAD/FABRICATION/JLCPCB/EMBARCADOS - CURSO PCB - BOM (JLCPCB).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\EMBARCADOS - CURSO PCB\HARDWARE\KICAD\FABRICATION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\EMBARCADOS - CURSO PCB\HARDWARE\KICAD\FABRICATION\JLCPCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45C38DCA-0C54-4DA1-8A24-DD29DC55FBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA1F383-ED49-404C-8636-7F8DCD2385C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8610" yWindow="-18270" windowWidth="28590" windowHeight="16500" xr2:uid="{6FCA7A09-F83E-4A28-8166-65CFB80E2157}"/>
+    <workbookView xWindow="-2235" yWindow="-29715" windowWidth="43200" windowHeight="23985" xr2:uid="{6FCA7A09-F83E-4A28-8166-65CFB80E2157}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="118">
   <si>
     <t>Comment</t>
   </si>
@@ -387,6 +387,9 @@
   </si>
   <si>
     <t xml:space="preserve">C6071564 </t>
+  </si>
+  <si>
+    <t>C25819</t>
   </si>
 </sst>
 </file>
@@ -760,9 +763,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F5AE25-B7CE-4529-BB6A-BD5320314784}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -985,7 +993,7 @@
         <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>